<commit_message>
EPBDS-6480 Implement "Collect" for DT tables.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="5" r:id="rId1"/>
@@ -53,7 +53,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="G4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This is so-called Decision Table Header. It consists of the keyword "Rules" and table signature.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C5" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This is keyword "properties". Each row in the properties section contains a pair of a property name and a property value in consecutive cells. If you want to define several properties, do not forget to merge across all cells in column. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -95,6 +123,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="G6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition column header. Must start with "C".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
@@ -196,7 +252,122 @@
         </r>
       </text>
     </comment>
+    <comment ref="G7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition expression.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">As you can see condition uses parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">hour </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Table Header and parameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>that defines column data. When condition is evaluated for each row, the cell value from this row is assigned to vaparameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This return statement is performed for each row where all conditions have been satisfied. The parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> is substituted with a cell value from the rule row.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E10" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 0 till 11 o'clock then greeting is "Good Morning, World!"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +396,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="I11" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 12 till 17
+ o'clock then greeting is "Good Afternoon, World!"</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This is so-called Decision Table Header. It consists of the keyword "Rules" and table signature.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,6 +453,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="H18" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This is keyword "properties". Each row in the properties section contains a pair of a property name and a property value in consecutive cells. If you want to define several properties, do not forget to merge across all cells in column. </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C19" authorId="0" shapeId="0">
       <text>
         <r>
@@ -295,6 +509,48 @@
         </r>
       </text>
     </comment>
+    <comment ref="H19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition column header. Must start with "C".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C20" authorId="0" shapeId="0">
       <text>
         <r>
@@ -429,6 +685,140 @@
         </r>
       </text>
     </comment>
+    <comment ref="H20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition expression.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">As you can see condition uses parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">hour </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Table Header and parameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>that defines column data. When condition is evaluated for each row, the cell value from this row is assigned to vaparameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This return statement is performed for each row where all conditions have been satisfied. The parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> is substituted with a cell value from the rule row.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This return statement is performed for each row where all conditions have been satisfied. The parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> is substituted with a cell value from the rule row.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E23" authorId="1" shapeId="0">
       <text>
         <r>
@@ -457,6 +847,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="J23" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 0 till 11 o'clock then greeting is "Good Morning, World!"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K23" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 0 till 11 o'clock then greeting is "Good Morning, World!"</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E24" authorId="1" shapeId="0">
       <text>
         <r>
@@ -473,6 +891,36 @@
       </text>
     </comment>
     <comment ref="F24" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 12 till 17
+ o'clock then greeting is "Good Afternoon, World!"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J24" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 12 till 17
+ o'clock then greeting is "Good Afternoon, World!"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K24" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -871,7 +1319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="105">
   <si>
     <t>Rule</t>
   </si>
@@ -1472,6 +1920,446 @@
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> (String driverMaritalStatus, String driverAge)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRET1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRET2</t>
+  </si>
+  <si>
+    <t>Rules String[] GreetingTwoRet3 (Integer hour)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>0 - 17</t>
+  </si>
+  <si>
+    <t>18 - 23</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Object[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Object[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting15 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting19 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting23 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
     </r>
   </si>
 </sst>
@@ -1563,18 +2451,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2132,252 +3014,255 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="34" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="26" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="29" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="41" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="41" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="43" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2781,8 +3666,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2793,9 +3678,12 @@
     <col min="4" max="4" width="19" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="63.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="42.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="49.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="3" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="53.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="35.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1">
@@ -2818,168 +3706,224 @@
     <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1">
+      <c r="G4" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="79"/>
+      <c r="I4" s="80"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="22.5" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="36" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="40" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="G9" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" ht="13.5" thickTop="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="42">
+      <c r="C10" s="41">
         <v>0</v>
       </c>
       <c r="D10" s="6">
         <v>11</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="42" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="G10" s="41">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>11</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="44">
+      <c r="C11" s="43">
         <v>12</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="44">
         <v>17</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="45" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="G11" s="43">
+        <v>0</v>
+      </c>
+      <c r="H11" s="44">
+        <v>17</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="44">
+      <c r="C12" s="43">
         <v>18</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D12" s="44">
         <v>21</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="45" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="G12" s="43">
+        <v>18</v>
+      </c>
+      <c r="H12" s="44">
+        <v>23</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="13.5" thickBot="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="47">
+      <c r="C13" s="46">
         <v>22</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="47">
         <v>23</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="48" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="46">
+        <v>22</v>
+      </c>
+      <c r="H13" s="47">
+        <v>23</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1">
       <c r="A14" s="5"/>
@@ -2994,98 +3938,160 @@
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1"/>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="17" spans="1:9" s="5" customFormat="1">
-      <c r="C17" s="77" t="s">
+    <row r="17" spans="1:11" s="5" customFormat="1">
+      <c r="C17" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="79"/>
-    </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="25.5">
-      <c r="C18" s="36" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80"/>
+      <c r="H17" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="80"/>
+    </row>
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="114.75">
+      <c r="C18" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="36" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1">
-      <c r="C19" s="36" t="s">
+      <c r="H18" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="5" customFormat="1">
+      <c r="C19" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="37" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="5" customFormat="1">
-      <c r="C20" s="36" t="s">
+      <c r="H19" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="5" customFormat="1">
+      <c r="C20" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1">
+      <c r="H20" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="37" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H21" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="13.5" thickBot="1">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="40" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" ht="13.5" thickTop="1">
+      <c r="H22" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="13.5" thickTop="1">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="42">
+      <c r="C23" s="41">
         <v>0</v>
       </c>
       <c r="D23" s="6">
@@ -3094,60 +4100,95 @@
       <c r="E23" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="43"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1">
+      <c r="H23" s="41">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6">
+        <v>11</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="42"/>
+    </row>
+    <row r="24" spans="1:11" s="3" customFormat="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="44">
+      <c r="C24" s="43">
         <v>12</v>
       </c>
-      <c r="D24" s="45">
+      <c r="D24" s="44">
         <v>17</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="46" t="s">
+      <c r="E24" s="33"/>
+      <c r="F24" s="45" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1">
+      <c r="H24" s="43">
+        <v>0</v>
+      </c>
+      <c r="I24" s="44">
+        <v>17</v>
+      </c>
+      <c r="J24" s="33"/>
+      <c r="K24" s="45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="3" customFormat="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="44">
+      <c r="C25" s="43">
         <v>18</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="44">
         <v>21</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="46"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H25" s="43">
+        <v>18</v>
+      </c>
+      <c r="I25" s="44">
+        <v>23</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="45"/>
+    </row>
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="47">
+      <c r="C26" s="46">
         <v>22</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="47">
         <v>23</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="49" t="s">
+      <c r="E26" s="49"/>
+      <c r="F26" s="48" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1">
+      <c r="H26" s="46">
+        <v>22</v>
+      </c>
+      <c r="I26" s="47">
+        <v>23</v>
+      </c>
+      <c r="J26" s="49"/>
+      <c r="K26" s="48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="3" customFormat="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3157,7 +4198,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1">
+    <row r="28" spans="1:11" s="3" customFormat="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3167,165 +4208,132 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" ht="15.75">
+    </row>
+    <row r="30" spans="1:11" s="3" customFormat="1" ht="15.75">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="78"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1">
+      <c r="D30" s="79"/>
+      <c r="E30" s="80"/>
+    </row>
+    <row r="31" spans="1:11" s="3" customFormat="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" s="3" customFormat="1">
+    </row>
+    <row r="32" spans="1:11" s="3" customFormat="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="E32" s="37"/>
     </row>
     <row r="33" spans="1:8" s="3" customFormat="1">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="41" t="s">
+      <c r="E34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" s="3" customFormat="1" ht="13.5" thickTop="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="41" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="51">
+      <c r="E35" s="50">
         <v>700</v>
       </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:8" s="3" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="51">
         <v>720</v>
       </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:8" s="3" customFormat="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="52">
+      <c r="E37" s="51">
         <v>300</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" s="3" customFormat="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="45" t="s">
+      <c r="D38" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="52">
+      <c r="E38" s="51">
         <v>350</v>
       </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="26"/>
     </row>
     <row r="39" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="53" t="s">
+      <c r="C39" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="55">
+      <c r="D39" s="53"/>
+      <c r="E39" s="54">
         <v>500</v>
       </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:8" s="3" customFormat="1">
       <c r="A40" s="5"/>
@@ -3335,7 +4343,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="26"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" s="3" customFormat="1">
       <c r="A41" s="5"/>
@@ -3345,7 +4353,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="26"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A42" s="5"/>
@@ -3355,184 +4363,172 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="26"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" s="3" customFormat="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="77" t="s">
+      <c r="C43" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="79"/>
+      <c r="D43" s="79"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="26"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" s="3" customFormat="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="38" t="s">
+      <c r="F44" s="37" t="s">
         <v>76</v>
       </c>
       <c r="G44" s="5"/>
-      <c r="H44" s="26"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" s="5" customFormat="1">
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="38"/>
-      <c r="H45" s="26"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="37"/>
     </row>
     <row r="46" spans="1:8" s="2" customFormat="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="38"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="37"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="26"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" s="2" customFormat="1" ht="13.5" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="40" t="s">
+      <c r="D47" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E47" s="33" t="s">
+      <c r="E47" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="41" t="s">
+      <c r="F47" s="40" t="s">
         <v>39</v>
       </c>
       <c r="G47" s="5"/>
-      <c r="H47" s="26"/>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" s="5" customFormat="1" ht="13.5" thickTop="1">
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="41" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="35">
+      <c r="E48" s="34">
         <v>700</v>
       </c>
-      <c r="F48" s="51">
+      <c r="F48" s="50">
         <v>700</v>
       </c>
-      <c r="H48" s="26"/>
     </row>
     <row r="49" spans="1:15" s="5" customFormat="1">
-      <c r="C49" s="44" t="s">
+      <c r="C49" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="45" t="s">
+      <c r="D49" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="52">
+      <c r="E49" s="34"/>
+      <c r="F49" s="51">
         <v>720</v>
       </c>
-      <c r="H49" s="26"/>
     </row>
     <row r="50" spans="1:15" s="5" customFormat="1">
-      <c r="C50" s="44" t="s">
+      <c r="C50" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D50" s="45" t="s">
+      <c r="D50" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="35">
+      <c r="E50" s="34">
         <v>300</v>
       </c>
-      <c r="F50" s="52"/>
-      <c r="H50" s="26"/>
+      <c r="F50" s="51"/>
     </row>
     <row r="51" spans="1:15" s="5" customFormat="1">
-      <c r="C51" s="44" t="s">
+      <c r="C51" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="45" t="s">
+      <c r="D51" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="35"/>
-      <c r="F51" s="52">
+      <c r="E51" s="34"/>
+      <c r="F51" s="51">
         <v>350</v>
       </c>
-      <c r="H51" s="26"/>
     </row>
     <row r="52" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="C52" s="47" t="s">
+      <c r="C52" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="48"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57">
+      <c r="D52" s="47"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="56">
         <v>500</v>
       </c>
-      <c r="H52" s="26"/>
-    </row>
-    <row r="53" spans="1:15" s="5" customFormat="1">
-      <c r="H53" s="26"/>
-    </row>
-    <row r="54" spans="1:15" s="5" customFormat="1">
-      <c r="H54" s="26"/>
-    </row>
-    <row r="55" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="H55" s="26"/>
-    </row>
+    </row>
+    <row r="53" spans="1:15" s="5" customFormat="1"/>
+    <row r="54" spans="1:15" s="5" customFormat="1"/>
+    <row r="55" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1"/>
     <row r="56" spans="1:15" s="2" customFormat="1" ht="15.75">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="77" t="s">
+      <c r="C56" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="78"/>
-      <c r="E56" s="78"/>
-      <c r="F56" s="79"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="80"/>
       <c r="G56" s="5"/>
-      <c r="H56" s="26"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
-      <c r="C57" s="36" t="s">
+      <c r="C57" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E57" s="31" t="s">
+      <c r="E57" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F57" s="38" t="s">
+      <c r="F57" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G57" s="5"/>
-      <c r="H57" s="26"/>
+      <c r="H57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
@@ -3540,118 +4536,109 @@
     <row r="58" spans="1:15" s="2" customFormat="1">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="31" t="s">
+      <c r="C58" s="35"/>
+      <c r="D58" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E58" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F58" s="38"/>
+      <c r="F58" s="37"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="26"/>
+      <c r="H58" s="5"/>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
     </row>
     <row r="59" spans="1:15" s="5" customFormat="1">
-      <c r="C59" s="36"/>
-      <c r="D59" s="31" t="s">
+      <c r="C59" s="35"/>
+      <c r="D59" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E59" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F59" s="38"/>
-      <c r="H59" s="26"/>
+      <c r="F59" s="37"/>
     </row>
     <row r="60" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="E60" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="F60" s="41" t="s">
+      <c r="F60" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:15" s="5" customFormat="1" ht="13.5" thickTop="1">
-      <c r="C61" s="58" t="s">
+      <c r="C61" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="80" t="s">
+      <c r="D61" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="E61" s="29" t="s">
+      <c r="E61" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="59">
+      <c r="F61" s="58">
         <v>700</v>
       </c>
-      <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:15" s="5" customFormat="1">
-      <c r="C62" s="60" t="s">
+      <c r="C62" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="81"/>
-      <c r="E62" s="28" t="s">
+      <c r="D62" s="82"/>
+      <c r="E62" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F62" s="61">
+      <c r="F62" s="60">
         <v>720</v>
       </c>
-      <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:15" s="5" customFormat="1">
-      <c r="C63" s="60" t="s">
+      <c r="C63" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D63" s="81" t="s">
+      <c r="D63" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="28" t="s">
+      <c r="E63" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="61">
+      <c r="F63" s="60">
         <v>300</v>
       </c>
-      <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:15" s="5" customFormat="1">
-      <c r="C64" s="60" t="s">
+      <c r="C64" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="28" t="s">
+      <c r="D64" s="82"/>
+      <c r="E64" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F64" s="61">
+      <c r="F64" s="60">
         <v>350</v>
       </c>
-      <c r="H64" s="26"/>
     </row>
     <row r="65" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="C65" s="62" t="s">
+      <c r="C65" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="64">
+      <c r="E65" s="62"/>
+      <c r="F65" s="63">
         <v>500</v>
       </c>
-      <c r="H65" s="26"/>
-    </row>
-    <row r="66" spans="1:14" s="5" customFormat="1">
-      <c r="H66" s="26"/>
-    </row>
+    </row>
+    <row r="66" spans="1:14" s="5" customFormat="1"/>
     <row r="67" spans="1:14">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
@@ -3660,7 +4647,7 @@
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
-      <c r="H67" s="26"/>
+      <c r="H67" s="5"/>
     </row>
     <row r="68" spans="1:14" ht="13.5" thickBot="1">
       <c r="A68" s="5"/>
@@ -3670,114 +4657,114 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
-      <c r="H68" s="26"/>
+      <c r="H68" s="5"/>
     </row>
     <row r="69" spans="1:14" ht="15.75">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="77" t="s">
+      <c r="C69" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="78"/>
-      <c r="E69" s="79"/>
+      <c r="D69" s="79"/>
+      <c r="E69" s="80"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
-      <c r="H69" s="26"/>
+      <c r="H69" s="5"/>
     </row>
     <row r="70" spans="1:14" ht="13.5" thickBot="1">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="39" t="s">
+      <c r="C70" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="41" t="s">
+      <c r="E70" s="40" t="s">
         <v>39</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
-      <c r="H70" s="26"/>
+      <c r="H70" s="5"/>
     </row>
     <row r="71" spans="1:14" ht="13.5" thickTop="1">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="42" t="s">
+      <c r="C71" s="41" t="s">
         <v>18</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="51">
+      <c r="E71" s="50">
         <v>700</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
-      <c r="H71" s="26"/>
+      <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
-      <c r="C72" s="44" t="s">
+      <c r="C72" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D72" s="45" t="s">
+      <c r="D72" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E72" s="52">
+      <c r="E72" s="51">
         <v>720</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
-      <c r="H72" s="26"/>
+      <c r="H72" s="5"/>
     </row>
     <row r="73" spans="1:14">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="44" t="s">
+      <c r="C73" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="45" t="s">
+      <c r="D73" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="52">
+      <c r="E73" s="51">
         <v>300</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
-      <c r="H73" s="26"/>
+      <c r="H73" s="5"/>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="44" t="s">
+      <c r="C74" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D74" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E74" s="52">
+      <c r="E74" s="51">
         <v>350</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
-      <c r="H74" s="26"/>
+      <c r="H74" s="5"/>
       <c r="N74" s="4"/>
     </row>
     <row r="75" spans="1:14" ht="13.5" thickBot="1">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="53" t="s">
+      <c r="C75" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D75" s="54"/>
-      <c r="E75" s="55">
+      <c r="D75" s="53"/>
+      <c r="E75" s="54">
         <v>500</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
-      <c r="H75" s="26"/>
+      <c r="H75" s="5"/>
       <c r="N75" s="4"/>
     </row>
     <row r="76" spans="1:14">
@@ -3788,38 +4775,38 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
-      <c r="H76" s="26"/>
+      <c r="H76" s="5"/>
       <c r="N76" s="3"/>
     </row>
     <row r="77" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1"/>
     <row r="78" spans="1:14" s="5" customFormat="1" ht="15.75">
-      <c r="C78" s="77" t="s">
+      <c r="C78" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="78"/>
-      <c r="E78" s="79"/>
+      <c r="D78" s="79"/>
+      <c r="E78" s="80"/>
     </row>
     <row r="79" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1">
-      <c r="C79" s="39" t="s">
+      <c r="C79" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="40" t="s">
+      <c r="D79" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="41" t="s">
+      <c r="E79" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="13.5" thickTop="1">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
-      <c r="C80" s="42" t="s">
+      <c r="C80" s="41" t="s">
         <v>18</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E80" s="51">
+      <c r="E80" s="50">
         <v>700</v>
       </c>
       <c r="F80" s="5"/>
@@ -3831,13 +4818,13 @@
     <row r="81" spans="1:13">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="44" t="s">
+      <c r="C81" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D81" s="45" t="s">
+      <c r="D81" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E81" s="52">
+      <c r="E81" s="51">
         <v>720</v>
       </c>
       <c r="F81" s="5"/>
@@ -3849,13 +4836,13 @@
     <row r="82" spans="1:13">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
-      <c r="C82" s="44" t="s">
+      <c r="C82" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D82" s="45" t="s">
+      <c r="D82" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E82" s="52">
+      <c r="E82" s="51">
         <v>300</v>
       </c>
       <c r="F82" s="5"/>
@@ -3867,13 +4854,13 @@
     <row r="83" spans="1:13">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="44" t="s">
+      <c r="C83" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="45" t="s">
+      <c r="D83" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="E83" s="52">
+      <c r="E83" s="51">
         <v>350</v>
       </c>
       <c r="F83" s="5"/>
@@ -3886,11 +4873,11 @@
     <row r="84" spans="1:13" ht="13.5" thickBot="1">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
-      <c r="C84" s="53" t="s">
+      <c r="C84" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D84" s="54"/>
-      <c r="E84" s="55">
+      <c r="D84" s="53"/>
+      <c r="E84" s="54">
         <v>500</v>
       </c>
       <c r="F84" s="5"/>
@@ -4074,16 +5061,18 @@
       <c r="J132" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="H17:K17"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="D61:D62"/>
     <mergeCell ref="D63:D64"/>
     <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C43:F43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4111,196 +5100,196 @@
   <sheetData>
     <row r="5" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="6" spans="3:5" ht="15.75">
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7" spans="3:5">
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:5">
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="3:5">
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="3:5" ht="12" customHeight="1" thickBot="1">
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="66" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="13.5" thickTop="1">
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="43" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="19">
         <v>700</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="58">
         <v>720</v>
       </c>
     </row>
     <row r="12" spans="3:5">
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="10">
         <v>300</v>
       </c>
-      <c r="E12" s="61">
+      <c r="E12" s="60">
         <v>350</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="13.5" thickBot="1">
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="84">
+      <c r="D13" s="86">
         <v>500</v>
       </c>
-      <c r="E13" s="85"/>
+      <c r="E13" s="87"/>
     </row>
     <row r="16" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="17" spans="3:9" ht="15.75">
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="79"/>
-      <c r="G17" s="77" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="80"/>
+      <c r="G17" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
     </row>
     <row r="18" spans="3:9" ht="26.25" thickBot="1">
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="66" t="s">
+      <c r="H18" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="67" t="s">
+      <c r="I18" s="66" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:9" ht="13.5" thickTop="1">
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="43" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="19">
         <v>700</v>
       </c>
-      <c r="E19" s="59">
+      <c r="E19" s="58">
         <v>720</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="43" t="s">
         <v>18</v>
       </c>
       <c r="H19" s="19">
         <v>700</v>
       </c>
-      <c r="I19" s="59">
+      <c r="I19" s="58">
         <v>720</v>
       </c>
     </row>
     <row r="20" spans="3:9">
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="43" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="10">
         <v>300</v>
       </c>
-      <c r="E20" s="61">
+      <c r="E20" s="60">
         <v>350</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="43" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="10">
         <v>300</v>
       </c>
-      <c r="I20" s="61">
+      <c r="I20" s="60">
         <v>350</v>
       </c>
     </row>
     <row r="21" spans="3:9" ht="13.5" thickBot="1">
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="84">
+      <c r="D21" s="86">
         <v>500</v>
       </c>
-      <c r="E21" s="85"/>
-      <c r="G21" s="47" t="s">
+      <c r="E21" s="87"/>
+      <c r="G21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="84">
+      <c r="H21" s="86">
         <v>500</v>
       </c>
-      <c r="I21" s="85"/>
+      <c r="I21" s="87"/>
     </row>
     <row r="25" spans="3:9" ht="15.75">
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
     </row>
     <row r="26" spans="3:9">
-      <c r="C26" s="82" t="s">
+      <c r="C26" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83" t="s">
+      <c r="E26" s="85"/>
+      <c r="F26" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="83"/>
+      <c r="G26" s="85"/>
     </row>
     <row r="27" spans="3:9" ht="13.5" thickBot="1">
-      <c r="C27" s="82"/>
+      <c r="C27" s="84"/>
       <c r="D27" s="18" t="s">
         <v>44</v>
       </c>
@@ -4369,7 +5358,7 @@
       <c r="C31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="29">
         <v>90400</v>
       </c>
       <c r="E31" s="21">
@@ -4384,29 +5373,29 @@
     </row>
     <row r="32" spans="3:9" ht="13.5" thickTop="1"/>
     <row r="34" spans="3:7" ht="15.75">
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
     </row>
     <row r="35" spans="3:7">
-      <c r="C35" s="82" t="s">
+      <c r="C35" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="83" t="s">
+      <c r="D35" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83" t="s">
+      <c r="E35" s="85"/>
+      <c r="F35" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="83"/>
+      <c r="G35" s="85"/>
     </row>
     <row r="36" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C36" s="82"/>
+      <c r="C36" s="84"/>
       <c r="D36" s="18" t="s">
         <v>44</v>
       </c>
@@ -4475,7 +5464,7 @@
       <c r="C40" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="30">
+      <c r="D40" s="29">
         <v>90400</v>
       </c>
       <c r="E40" s="21">
@@ -4491,6 +5480,11 @@
     <row r="41" spans="3:7" ht="13.5" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C25:G25"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:E35"/>
@@ -4500,11 +5494,6 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4513,10 +5502,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:J54"/>
+  <dimension ref="C4:M105"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:G37"/>
+    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4526,35 +5515,37 @@
     <col min="5" max="5" width="24.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="33.85546875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="13.5" thickBot="1"/>
     <row r="5" spans="3:10" ht="15.75">
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="80"/>
     </row>
     <row r="6" spans="3:10">
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="67" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="14">
@@ -4566,18 +5557,18 @@
       <c r="I6" s="15">
         <v>18</v>
       </c>
-      <c r="J6" s="69">
+      <c r="J6" s="68">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="3:10" ht="13.5" thickBot="1">
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="23" t="s">
@@ -4592,12 +5583,12 @@
       <c r="I7" s="15">
         <v>21</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="68">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="69" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -4606,7 +5597,7 @@
       <c r="E8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="24" t="s">
@@ -4618,337 +5609,1037 @@
       <c r="I8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="71" t="s">
+      <c r="J8" s="70" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="75"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="74"/>
     </row>
     <row r="12" spans="3:10" ht="13.5" thickBot="1"/>
     <row r="13" spans="3:10" ht="15.75">
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="80"/>
     </row>
     <row r="14" spans="3:10">
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="38" t="s">
+      <c r="D14" s="89"/>
+      <c r="E14" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="3:10">
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="88"/>
-      <c r="E15" s="38" t="s">
+      <c r="D15" s="89"/>
+      <c r="E15" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="3:10">
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="13.5" thickBot="1">
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="13.5" thickTop="1">
-      <c r="C18" s="42">
+      <c r="C18" s="41">
         <v>0</v>
       </c>
       <c r="D18" s="6">
         <v>11</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="42" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="44">
+      <c r="C19" s="43">
         <v>12</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="44">
         <v>17</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="3:5">
-      <c r="C20" s="44">
+      <c r="C20" s="43">
         <v>18</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="44">
         <v>21</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="45" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="13.5" thickBot="1">
-      <c r="C21" s="47">
+      <c r="C21" s="46">
         <v>22</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="47">
         <v>23</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="48" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="25" spans="3:5" ht="15.75">
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="79"/>
+      <c r="D25" s="80"/>
     </row>
     <row r="26" spans="3:5">
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="38" t="s">
+      <c r="D26" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="3:5">
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="3:5">
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="13.5" thickBot="1">
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="13.5" thickTop="1">
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="42" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="3:5">
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="3:5">
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C33" s="76" t="s">
+    <row r="33" spans="3:13" ht="13.5" thickBot="1">
+      <c r="C33" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="48" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="13.5" thickBot="1"/>
-    <row r="37" spans="3:7" ht="15.75">
-      <c r="C37" s="77" t="s">
+    <row r="36" spans="3:13" ht="13.5" thickBot="1"/>
+    <row r="37" spans="3:13" ht="15.75">
+      <c r="C37" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="79"/>
-      <c r="F37" s="77" t="s">
+      <c r="D37" s="80"/>
+      <c r="F37" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="79"/>
-    </row>
-    <row r="38" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C38" s="39" t="s">
+      <c r="G37" s="80"/>
+      <c r="I37" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37" s="80"/>
+      <c r="L37" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="M37" s="80"/>
+    </row>
+    <row r="38" spans="3:13" ht="13.5" thickBot="1">
+      <c r="C38" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="41" t="s">
+      <c r="G38" s="40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="3:7" ht="13.5" thickTop="1">
-      <c r="C39" s="42" t="s">
+      <c r="I38" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J38" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" ht="13.5" thickTop="1">
+      <c r="C39" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="43" t="s">
+      <c r="G39" s="42" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="3:7">
-      <c r="C40" s="44" t="s">
+      <c r="I39" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="L39" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="M39" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13">
+      <c r="C40" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="44" t="s">
+      <c r="F40" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="46" t="s">
+      <c r="G40" s="45" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="3:7">
-      <c r="C41" s="44" t="s">
+      <c r="I40" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="L40" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="M40" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13">
+      <c r="C41" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="46" t="s">
+      <c r="D41" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F41" s="44" t="s">
+      <c r="F41" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="46" t="s">
+      <c r="G41" s="45" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C42" s="76" t="s">
+      <c r="I41" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="L41" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="M41" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13" ht="13.5" thickBot="1">
+      <c r="C42" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="76" t="s">
+      <c r="F42" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="G42" s="49" t="s">
+      <c r="G42" s="48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="3:7" ht="13.5" thickBot="1"/>
-    <row r="46" spans="3:7" ht="15.75">
-      <c r="C46" s="77" t="s">
+      <c r="I42" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="L42" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="M42" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" ht="13.5" thickBot="1"/>
+    <row r="46" spans="3:13" ht="15.75">
+      <c r="C46" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="79"/>
-    </row>
-    <row r="47" spans="3:7">
-      <c r="C47" s="36" t="s">
+      <c r="D46" s="80"/>
+      <c r="F46" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="G46" s="80"/>
+      <c r="I46" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="80"/>
+    </row>
+    <row r="47" spans="3:13" ht="13.5" thickBot="1">
+      <c r="C47" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D47" s="37" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="48" spans="3:7" ht="25.5">
-      <c r="C48" s="36" t="s">
+      <c r="F47" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J47" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13" ht="26.25" thickTop="1">
+      <c r="C48" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="36" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="3:4">
-      <c r="C49" s="36" t="s">
+      <c r="F48" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J48" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10">
+      <c r="C49" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D49" s="37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="3:4" ht="13.5" thickBot="1">
-      <c r="C50" s="39" t="s">
+      <c r="F49" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I49" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J49" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" ht="13.5" thickBot="1">
+      <c r="C50" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D50" s="41" t="s">
+      <c r="D50" s="40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="51" spans="3:4" ht="13.5" thickTop="1">
-      <c r="C51" s="42" t="s">
+      <c r="F50" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="I50" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J50" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
+      <c r="C51" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="3:4">
-      <c r="C52" s="44" t="s">
+      <c r="F51" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I51" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J51" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10">
+      <c r="C52" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="46" t="s">
+      <c r="D52" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="3:4">
-      <c r="C53" s="44" t="s">
+    <row r="53" spans="3:10">
+      <c r="C53" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="46" t="s">
+      <c r="D53" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="3:4" ht="13.5" thickBot="1">
-      <c r="C54" s="76" t="s">
+    <row r="54" spans="3:10" ht="13.5" thickBot="1">
+      <c r="C54" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="49" t="s">
+      <c r="D54" s="48" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="55" spans="3:10" ht="15.75">
+      <c r="F55" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="G55" s="80"/>
+      <c r="I55" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="J55" s="80"/>
+    </row>
+    <row r="56" spans="3:10" ht="13.5" thickBot="1">
+      <c r="F56" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G56" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J56" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" ht="13.5" thickTop="1">
+      <c r="F57" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J57" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10">
+      <c r="F58" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I58" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J58" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10">
+      <c r="F59" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G59" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="I59" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J59" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" ht="13.5" thickBot="1">
+      <c r="F60" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G60" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I60" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J60" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" ht="13.5" thickBot="1"/>
+    <row r="64" spans="3:10" ht="15.75">
+      <c r="F64" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="G64" s="80"/>
+      <c r="I64" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="J64" s="80"/>
+    </row>
+    <row r="65" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F65" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G65" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I65" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J65" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="6:10" ht="13.5" thickTop="1">
+      <c r="F66" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G66" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I66" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J66" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="6:10">
+      <c r="F67" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G67" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I67" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J67" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="6:10">
+      <c r="F68" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G68" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="I68" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J68" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F69" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G69" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I69" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J69" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="6:10" ht="13.5" thickBot="1"/>
+    <row r="73" spans="6:10" ht="15.75">
+      <c r="F73" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" s="80"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="J73" s="80"/>
+    </row>
+    <row r="74" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F74" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G74" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" s="3"/>
+      <c r="I74" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J74" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="6:10" ht="13.5" thickTop="1">
+      <c r="F75" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G75" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H75" s="3"/>
+      <c r="I75" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J75" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="6:10">
+      <c r="F76" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G76" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" s="3"/>
+      <c r="I76" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J76" s="45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="6:10">
+      <c r="F77" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G77" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H77" s="3"/>
+      <c r="I77" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J77" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F78" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G78" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="H78" s="3"/>
+      <c r="I78" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J78" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="6:10">
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="6:10">
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="6:10" ht="15.75">
+      <c r="F82" s="78" t="s">
+        <v>98</v>
+      </c>
+      <c r="G82" s="80"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J82" s="80"/>
+    </row>
+    <row r="83" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F83" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G83" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="3"/>
+      <c r="I83" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J83" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="6:10" ht="13.5" thickTop="1">
+      <c r="F84" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G84" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H84" s="3"/>
+      <c r="I84" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J84" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="6:10">
+      <c r="F85" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G85" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="H85" s="3"/>
+      <c r="I85" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J85" s="45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="6:10">
+      <c r="F86" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G86" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H86" s="3"/>
+      <c r="I86" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J86" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="87" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F87" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G87" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="H87" s="3"/>
+      <c r="I87" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J87" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="6:10" ht="13.5" thickBot="1"/>
+    <row r="91" spans="6:10" ht="15.75">
+      <c r="F91" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="G91" s="80"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="J91" s="80"/>
+    </row>
+    <row r="92" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F92" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G92" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H92" s="3"/>
+      <c r="I92" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J92" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="6:10" ht="13.5" thickTop="1">
+      <c r="F93" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G93" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H93" s="3"/>
+      <c r="I93" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J93" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="6:10">
+      <c r="F94" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G94" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="H94" s="3"/>
+      <c r="I94" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J94" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="6:10">
+      <c r="F95" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G95" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H95" s="3"/>
+      <c r="I95" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J95" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F96" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G96" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="H96" s="3"/>
+      <c r="I96" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J96" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="6:10">
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="6:10">
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="6:10" ht="15.75">
+      <c r="F100" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="G100" s="80"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="78" t="s">
+        <v>103</v>
+      </c>
+      <c r="J100" s="80"/>
+    </row>
+    <row r="101" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F101" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G101" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H101" s="3"/>
+      <c r="I101" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J101" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="6:10" ht="13.5" thickTop="1">
+      <c r="F102" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G102" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="H102" s="3"/>
+      <c r="I102" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J102" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="6:10">
+      <c r="F103" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G103" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="H103" s="3"/>
+      <c r="I103" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="J103" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="6:10">
+      <c r="F104" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="G104" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H104" s="3"/>
+      <c r="I104" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J104" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="105" spans="6:10" ht="13.5" thickBot="1">
+      <c r="F105" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="G105" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="H105" s="3"/>
+      <c r="I105" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="J105" s="48" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="24">
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="I55:J55"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="C13:E13"/>
@@ -4957,6 +6648,7 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-6590 Only the first condition is taken in complex rules
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="5" r:id="rId1"/>
@@ -992,6 +992,163 @@
         </r>
       </text>
     </comment>
+    <comment ref="H33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This is so-called Decision Table Header. It consists of the keyword "Rules" and table signature.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This is keyword "properties". Each row in the properties section contains a pair of a property name and a property value in consecutive cells. If you want to define several properties, do not forget to merge across all cells in column. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition column header. Must start with "C".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Return column header. Must start with "RET".  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Condition expression.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">As you can see condition uses parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">hour </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>from Table Header and parameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>that defines column data. When condition is evaluated for each row, the cell value from this row is assigned to vaparameter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve"> min.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J36" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">This return statement is performed for each row where all conditions have been satisfied. The parameter </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Courier New"/>
+            <family val="3"/>
+          </rPr>
+          <t>greeting</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve"> is substituted with a cell value from the rule row.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D39" authorId="1" shapeId="0">
       <text>
         <r>
@@ -1003,6 +1160,35 @@
             <charset val="204"/>
           </rPr>
           <t>Blank cell means any Marital status.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J39" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 0 till 11 o'clock then greeting is "Good Morning, World!"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J40" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>This rule is interpreted as if the hour from 12 till 17
+ o'clock then greeting is "Good Afternoon, World!"</t>
         </r>
       </text>
     </comment>
@@ -1319,7 +1505,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="107">
   <si>
     <t>Rule</t>
   </si>
@@ -2361,6 +2547,34 @@
       </rPr>
       <t xml:space="preserve"> (Integer hour)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting70</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>=null</t>
   </si>
 </sst>
 </file>
@@ -3014,7 +3228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3221,6 +3435,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3666,8 +3886,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3706,17 +3926,17 @@
     <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="79"/>
-      <c r="I4" s="80"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="22.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -3939,20 +4159,20 @@
     <row r="15" spans="1:9" s="5" customFormat="1"/>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="13.5" thickBot="1"/>
     <row r="17" spans="1:11" s="5" customFormat="1">
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="80"/>
-      <c r="H17" s="78" t="s">
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="82"/>
+      <c r="H17" s="80" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="80"/>
-    </row>
-    <row r="18" spans="1:11" s="5" customFormat="1" ht="114.75">
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="82"/>
+    </row>
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="25.5">
       <c r="C18" s="35" t="s">
         <v>29</v>
       </c>
@@ -4218,11 +4438,11 @@
     <row r="30" spans="1:11" s="3" customFormat="1" ht="15.75">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="78" t="s">
+      <c r="C30" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
     </row>
     <row r="31" spans="1:11" s="3" customFormat="1">
       <c r="A31" s="5"/>
@@ -4237,7 +4457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1">
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="35" t="s">
@@ -4248,7 +4468,7 @@
       </c>
       <c r="E32" s="37"/>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1">
+    <row r="33" spans="1:10" s="3" customFormat="1" ht="15.75">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="35" t="s">
@@ -4258,8 +4478,13 @@
         <v>35</v>
       </c>
       <c r="E33" s="37"/>
-    </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H33" s="80" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="81"/>
+      <c r="J33" s="82"/>
+    </row>
+    <row r="34" spans="1:10" s="3" customFormat="1" ht="26.25" thickBot="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="38" t="s">
@@ -4271,8 +4496,17 @@
       <c r="E34" s="40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" ht="13.5" thickTop="1">
+      <c r="H34" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="3" customFormat="1" ht="13.5" thickTop="1">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="41" t="s">
@@ -4284,8 +4518,17 @@
       <c r="E35" s="50">
         <v>700</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" s="3" customFormat="1">
+      <c r="H35" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="3" customFormat="1">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43" t="s">
@@ -4297,8 +4540,15 @@
       <c r="E36" s="51">
         <v>720</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" s="3" customFormat="1">
+      <c r="H36" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="37"/>
+    </row>
+    <row r="37" spans="1:10" s="3" customFormat="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="43" t="s">
@@ -4310,8 +4560,17 @@
       <c r="E37" s="51">
         <v>300</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" s="3" customFormat="1">
+      <c r="H37" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="J37" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="43" t="s">
@@ -4323,8 +4582,17 @@
       <c r="E38" s="51">
         <v>350</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H38" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="3" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="52" t="s">
@@ -4334,8 +4602,17 @@
       <c r="E39" s="54">
         <v>500</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" s="3" customFormat="1">
+      <c r="H39" s="41">
+        <v>0</v>
+      </c>
+      <c r="I39" s="6">
+        <v>11</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -4343,9 +4620,15 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" s="3" customFormat="1">
+      <c r="H40" s="43">
+        <v>0</v>
+      </c>
+      <c r="I40" s="44">
+        <v>17</v>
+      </c>
+      <c r="J40" s="45"/>
+    </row>
+    <row r="41" spans="1:10" s="3" customFormat="1">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -4353,9 +4636,17 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" s="3" customFormat="1" ht="13.5" thickBot="1">
+      <c r="H41" s="43">
+        <v>0</v>
+      </c>
+      <c r="I41" s="44">
+        <v>23</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="3" customFormat="1" ht="13.5" thickBot="1">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -4363,21 +4654,29 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" s="3" customFormat="1">
+      <c r="H42" s="46">
+        <v>22</v>
+      </c>
+      <c r="I42" s="47">
+        <v>23</v>
+      </c>
+      <c r="J42" s="48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="3" customFormat="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="78" t="s">
+      <c r="C43" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="80"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="82"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" s="3" customFormat="1">
+    <row r="44" spans="1:10" s="3" customFormat="1">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="35" t="s">
@@ -4395,7 +4694,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" s="5" customFormat="1">
+    <row r="45" spans="1:10" s="5" customFormat="1">
       <c r="C45" s="35" t="s">
         <v>15</v>
       </c>
@@ -4405,7 +4704,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="37"/>
     </row>
-    <row r="46" spans="1:8" s="2" customFormat="1">
+    <row r="46" spans="1:10" s="2" customFormat="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="35" t="s">
@@ -4419,7 +4718,7 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="13.5" thickBot="1">
+    <row r="47" spans="1:10" s="2" customFormat="1" ht="13.5" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="38" t="s">
@@ -4437,7 +4736,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" ht="13.5" thickTop="1">
+    <row r="48" spans="1:10" s="5" customFormat="1" ht="13.5" thickTop="1">
       <c r="C48" s="41" t="s">
         <v>18</v>
       </c>
@@ -4503,12 +4802,12 @@
     <row r="56" spans="1:15" s="2" customFormat="1" ht="15.75">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="78" t="s">
+      <c r="C56" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="80"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="82"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
@@ -4578,7 +4877,7 @@
       <c r="C61" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="81" t="s">
+      <c r="D61" s="83" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="28" t="s">
@@ -4592,7 +4891,7 @@
       <c r="C62" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="D62" s="82"/>
+      <c r="D62" s="84"/>
       <c r="E62" s="27" t="s">
         <v>20</v>
       </c>
@@ -4604,7 +4903,7 @@
       <c r="C63" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D63" s="84" t="s">
         <v>21</v>
       </c>
       <c r="E63" s="27" t="s">
@@ -4618,7 +4917,7 @@
       <c r="C64" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D64" s="82"/>
+      <c r="D64" s="84"/>
       <c r="E64" s="27" t="s">
         <v>20</v>
       </c>
@@ -4662,11 +4961,11 @@
     <row r="69" spans="1:14" ht="15.75">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="78" t="s">
+      <c r="C69" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="79"/>
-      <c r="E69" s="80"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="82"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
@@ -4780,11 +5079,11 @@
     </row>
     <row r="77" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1"/>
     <row r="78" spans="1:14" s="5" customFormat="1" ht="15.75">
-      <c r="C78" s="78" t="s">
+      <c r="C78" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="79"/>
-      <c r="E78" s="80"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="82"/>
     </row>
     <row r="79" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1">
       <c r="C79" s="38" t="s">
@@ -5061,13 +5360,14 @@
       <c r="J132" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H33:J33"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="D61:D62"/>
@@ -5100,11 +5400,11 @@
   <sheetData>
     <row r="5" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="6" spans="3:5" ht="15.75">
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="3:5">
       <c r="C7" s="35" t="s">
@@ -5172,23 +5472,23 @@
       <c r="C13" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="88">
         <v>500</v>
       </c>
-      <c r="E13" s="87"/>
+      <c r="E13" s="89"/>
     </row>
     <row r="16" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="17" spans="3:9" ht="15.75">
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="G17" s="78" t="s">
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="G17" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="79"/>
-      <c r="I17" s="80"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="82"/>
     </row>
     <row r="18" spans="3:9" ht="26.25" thickBot="1">
       <c r="C18" s="64" t="s">
@@ -5254,42 +5554,42 @@
       <c r="C21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="86">
+      <c r="D21" s="88">
         <v>500</v>
       </c>
-      <c r="E21" s="87"/>
+      <c r="E21" s="89"/>
       <c r="G21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="86">
+      <c r="H21" s="88">
         <v>500</v>
       </c>
-      <c r="I21" s="87"/>
+      <c r="I21" s="89"/>
     </row>
     <row r="25" spans="3:9" ht="15.75">
-      <c r="C25" s="83" t="s">
+      <c r="C25" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
     </row>
     <row r="26" spans="3:9">
-      <c r="C26" s="84" t="s">
+      <c r="C26" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="85" t="s">
+      <c r="D26" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85" t="s">
+      <c r="E26" s="87"/>
+      <c r="F26" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="85"/>
+      <c r="G26" s="87"/>
     </row>
     <row r="27" spans="3:9" ht="13.5" thickBot="1">
-      <c r="C27" s="84"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="18" t="s">
         <v>44</v>
       </c>
@@ -5373,29 +5673,29 @@
     </row>
     <row r="32" spans="3:9" ht="13.5" thickTop="1"/>
     <row r="34" spans="3:7" ht="15.75">
-      <c r="C34" s="83" t="s">
+      <c r="C34" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
     </row>
     <row r="35" spans="3:7">
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="85" t="s">
+      <c r="D35" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85" t="s">
+      <c r="E35" s="87"/>
+      <c r="F35" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="85"/>
+      <c r="G35" s="87"/>
     </row>
     <row r="36" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C36" s="84"/>
+      <c r="C36" s="86"/>
       <c r="D36" s="18" t="s">
         <v>44</v>
       </c>
@@ -5504,7 +5804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
+    <sheetView topLeftCell="B82" workbookViewId="0">
       <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
@@ -5524,16 +5824,16 @@
   <sheetData>
     <row r="4" spans="3:10" ht="13.5" thickBot="1"/>
     <row r="5" spans="3:10" ht="15.75">
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="80"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="35" t="s">
@@ -5625,26 +5925,26 @@
     </row>
     <row r="12" spans="3:10" ht="13.5" thickBot="1"/>
     <row r="13" spans="3:10" ht="15.75">
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82"/>
     </row>
     <row r="14" spans="3:10">
-      <c r="C14" s="88" t="s">
+      <c r="C14" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="89"/>
+      <c r="D14" s="91"/>
       <c r="E14" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="3:10">
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="89"/>
+      <c r="D15" s="91"/>
       <c r="E15" s="37" t="s">
         <v>14</v>
       </c>
@@ -5717,10 +6017,10 @@
     </row>
     <row r="24" spans="3:5" ht="13.5" thickBot="1"/>
     <row r="25" spans="3:5" ht="15.75">
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="80"/>
+      <c r="D25" s="82"/>
     </row>
     <row r="26" spans="3:5">
       <c r="C26" s="35" t="s">
@@ -5788,22 +6088,22 @@
     </row>
     <row r="36" spans="3:13" ht="13.5" thickBot="1"/>
     <row r="37" spans="3:13" ht="15.75">
-      <c r="C37" s="78" t="s">
+      <c r="C37" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="80"/>
-      <c r="F37" s="78" t="s">
+      <c r="D37" s="82"/>
+      <c r="F37" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="80"/>
-      <c r="I37" s="78" t="s">
+      <c r="G37" s="82"/>
+      <c r="I37" s="80" t="s">
         <v>87</v>
       </c>
-      <c r="J37" s="80"/>
-      <c r="L37" s="78" t="s">
+      <c r="J37" s="82"/>
+      <c r="L37" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="M37" s="80"/>
+      <c r="M37" s="82"/>
     </row>
     <row r="38" spans="3:13" ht="13.5" thickBot="1">
       <c r="C38" s="38" t="s">
@@ -5937,18 +6237,18 @@
     </row>
     <row r="45" spans="3:13" ht="13.5" thickBot="1"/>
     <row r="46" spans="3:13" ht="15.75">
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="80"/>
-      <c r="F46" s="78" t="s">
+      <c r="D46" s="82"/>
+      <c r="F46" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="G46" s="80"/>
-      <c r="I46" s="78" t="s">
+      <c r="G46" s="82"/>
+      <c r="I46" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="J46" s="80"/>
+      <c r="J46" s="82"/>
     </row>
     <row r="47" spans="3:13" ht="13.5" thickBot="1">
       <c r="C47" s="35" t="s">
@@ -6075,14 +6375,14 @@
       </c>
     </row>
     <row r="55" spans="3:10" ht="15.75">
-      <c r="F55" s="78" t="s">
+      <c r="F55" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="G55" s="80"/>
-      <c r="I55" s="78" t="s">
+      <c r="G55" s="82"/>
+      <c r="I55" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="J55" s="80"/>
+      <c r="J55" s="82"/>
     </row>
     <row r="56" spans="3:10" ht="13.5" thickBot="1">
       <c r="F56" s="38" t="s">
@@ -6156,14 +6456,14 @@
     </row>
     <row r="63" spans="3:10" ht="13.5" thickBot="1"/>
     <row r="64" spans="3:10" ht="15.75">
-      <c r="F64" s="78" t="s">
+      <c r="F64" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="G64" s="80"/>
-      <c r="I64" s="78" t="s">
+      <c r="G64" s="82"/>
+      <c r="I64" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J64" s="80"/>
+      <c r="J64" s="82"/>
     </row>
     <row r="65" spans="6:10" ht="13.5" thickBot="1">
       <c r="F65" s="38" t="s">
@@ -6237,15 +6537,15 @@
     </row>
     <row r="72" spans="6:10" ht="13.5" thickBot="1"/>
     <row r="73" spans="6:10" ht="15.75">
-      <c r="F73" s="78" t="s">
+      <c r="F73" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="G73" s="80"/>
+      <c r="G73" s="82"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="78" t="s">
+      <c r="I73" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="J73" s="80"/>
+      <c r="J73" s="82"/>
     </row>
     <row r="74" spans="6:10" ht="13.5" thickBot="1">
       <c r="F74" s="38" t="s">
@@ -6344,15 +6644,15 @@
       <c r="J81" s="3"/>
     </row>
     <row r="82" spans="6:10" ht="15.75">
-      <c r="F82" s="78" t="s">
+      <c r="F82" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="G82" s="80"/>
+      <c r="G82" s="82"/>
       <c r="H82" s="3"/>
-      <c r="I82" s="78" t="s">
+      <c r="I82" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="J82" s="80"/>
+      <c r="J82" s="82"/>
     </row>
     <row r="83" spans="6:10" ht="13.5" thickBot="1">
       <c r="F83" s="38" t="s">
@@ -6431,15 +6731,15 @@
     </row>
     <row r="90" spans="6:10" ht="13.5" thickBot="1"/>
     <row r="91" spans="6:10" ht="15.75">
-      <c r="F91" s="78" t="s">
+      <c r="F91" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="G91" s="80"/>
+      <c r="G91" s="82"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="78" t="s">
+      <c r="I91" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="J91" s="80"/>
+      <c r="J91" s="82"/>
     </row>
     <row r="92" spans="6:10" ht="13.5" thickBot="1">
       <c r="F92" s="38" t="s">
@@ -6538,15 +6838,15 @@
       <c r="J99" s="3"/>
     </row>
     <row r="100" spans="6:10" ht="15.75">
-      <c r="F100" s="78" t="s">
+      <c r="F100" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="G100" s="80"/>
+      <c r="G100" s="82"/>
       <c r="H100" s="3"/>
-      <c r="I100" s="78" t="s">
+      <c r="I100" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="J100" s="80"/>
+      <c r="J100" s="82"/>
     </row>
     <row r="101" spans="6:10" ht="13.5" thickBot="1">
       <c r="F101" s="38" t="s">

</xml_diff>

<commit_message>
EPBDS-7806 SmartLookups: inputs should be matched to the vertical conditions first, after that to horizontal conditions
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D079BE-C0D2-400D-8D8F-7C5E27D03192}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="5" r:id="rId1"/>
@@ -33,13 +34,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stanislav Shor</author>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="1" shapeId="0">
+    <comment ref="C5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="1" shapeId="0">
+    <comment ref="G5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -151,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -219,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -252,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -320,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -353,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="1" shapeId="0">
+    <comment ref="E10" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -367,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="1" shapeId="0">
+    <comment ref="I10" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="1" shapeId="0">
+    <comment ref="E11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -396,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="1" shapeId="0">
+    <comment ref="I11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -411,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="1" shapeId="0">
+    <comment ref="C18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -453,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="1" shapeId="0">
+    <comment ref="H18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -467,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -481,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0">
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -495,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -509,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -523,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0" shapeId="0">
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -537,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K19" authorId="0" shapeId="0">
+    <comment ref="K19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -551,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -619,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -652,7 +653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -685,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -753,7 +754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0" shapeId="0">
+    <comment ref="J20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -786,7 +787,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -819,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E23" authorId="1" shapeId="0">
+    <comment ref="E23" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -833,7 +834,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="1" shapeId="0">
+    <comment ref="F23" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -847,7 +848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="1" shapeId="0">
+    <comment ref="J23" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -861,7 +862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K23" authorId="1" shapeId="0">
+    <comment ref="K23" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -875,7 +876,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E24" authorId="1" shapeId="0">
+    <comment ref="E24" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -890,7 +891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="1" shapeId="0">
+    <comment ref="F24" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -905,7 +906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="1" shapeId="0">
+    <comment ref="J24" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -920,7 +921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K24" authorId="1" shapeId="0">
+    <comment ref="K24" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -935,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="1" shapeId="0">
+    <comment ref="C32" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -950,7 +951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="1" shapeId="0">
+    <comment ref="E32" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -964,7 +965,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="1" shapeId="0">
+    <comment ref="C33" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -978,7 +979,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="1" shapeId="0">
+    <comment ref="E33" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -992,7 +993,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H33" authorId="0" shapeId="0">
+    <comment ref="H33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1007,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H34" authorId="1" shapeId="0">
+    <comment ref="H34" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -1020,7 +1021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H35" authorId="0" shapeId="0">
+    <comment ref="H35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -1034,7 +1035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J35" authorId="0" shapeId="0">
+    <comment ref="J35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
       <text>
         <r>
           <rPr>
@@ -1048,7 +1049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H36" authorId="0" shapeId="0">
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
       <text>
         <r>
           <rPr>
@@ -1116,7 +1117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J36" authorId="0" shapeId="0">
+    <comment ref="J36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -1149,7 +1150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D39" authorId="1" shapeId="0">
+    <comment ref="D39" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000033000000}">
       <text>
         <r>
           <rPr>
@@ -1163,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J39" authorId="1" shapeId="0">
+    <comment ref="J39" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000034000000}">
       <text>
         <r>
           <rPr>
@@ -1177,7 +1178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J40" authorId="1" shapeId="0">
+    <comment ref="J40" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000035000000}">
       <text>
         <r>
           <rPr>
@@ -1192,7 +1193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="1" shapeId="0">
+    <comment ref="C45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000036000000}">
       <text>
         <r>
           <rPr>
@@ -1207,7 +1208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E45" authorId="1" shapeId="0">
+    <comment ref="E45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000037000000}">
       <text>
         <r>
           <rPr>
@@ -1221,7 +1222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="1" shapeId="0">
+    <comment ref="F45" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000038000000}">
       <text>
         <r>
           <rPr>
@@ -1235,7 +1236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="1" shapeId="0">
+    <comment ref="C46" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000039000000}">
       <text>
         <r>
           <rPr>
@@ -1249,7 +1250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E46" authorId="1" shapeId="0">
+    <comment ref="E46" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -1263,7 +1264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="1" shapeId="0">
+    <comment ref="F46" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -1277,7 +1278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D52" authorId="1" shapeId="0">
+    <comment ref="D52" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -1291,7 +1292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -1305,7 +1306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D61" authorId="1" shapeId="0">
+    <comment ref="D61" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -1324,12 +1325,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1357,7 +1358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1371,7 +1372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1385,7 +1386,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1399,7 +1400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="0" shapeId="0">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1413,7 +1414,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="0" shapeId="0">
+    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">The height of the first column title cell = Number of horizontal conditions </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{80289188-E1BF-4C97-9B39-AC509D1F260D}">
       <text>
         <r>
           <rPr>
@@ -1432,12 +1447,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Elena Poyasok</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1451,7 +1466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0" shapeId="0">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1465,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0" shapeId="0">
+    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1505,7 +1520,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="109">
   <si>
     <t>Rule</t>
   </si>
@@ -2060,6 +2075,499 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">SmartRules DoubleValue </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>DriverPremium7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverMaritalStatus, String driverAge)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRET1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRET2</t>
+  </si>
+  <si>
+    <t>Rules String[] GreetingTwoRet3 (Integer hour)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>0 - 17</t>
+  </si>
+  <si>
+    <t>18 - 23</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect String[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Object[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Object[] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Collection </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting15 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting19 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect as String List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartRules Collect as String List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Greeting23 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SimpleRules Collect List </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules String </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Greeting70</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>=null</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">SmartLookup DoubleValue </t>
     </r>
     <r>
@@ -2080,12 +2588,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> ( String driverAge, String name, String driverdriverMaritalStatus)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules DoubleValue </t>
+      <t xml:space="preserve"> ( String driverAge, String name, String mStatus)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartLookup DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -2095,7 +2603,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>DriverPremium7</t>
+      <t>DriverPremium8</t>
     </r>
     <r>
       <rPr>
@@ -2105,15 +2613,12 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (String driverMaritalStatus, String driverAge)</t>
-    </r>
-  </si>
-  <si>
-    <t>CRET1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules String[] </t>
+      <t xml:space="preserve"> (String name, String mStatus, String driverAge)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmartLookup DoubleValue </t>
     </r>
     <r>
       <rPr>
@@ -2123,7 +2628,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t>Greeting7</t>
+      <t>CarPrice3</t>
     </r>
     <r>
       <rPr>
@@ -2133,460 +2638,20 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <t>CRET2</t>
-  </si>
-  <si>
-    <t>Rules String[] GreetingTwoRet3 (Integer hour)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect String[] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <t>0 - 17</t>
-  </si>
-  <si>
-    <t>18 - 23</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules Collect String[] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules Collect as String Object[] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect as String Object[] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect as String Collection </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules Collect as String Collection </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect Collection </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect Collection </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Greeting15 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect as String Set </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect Set </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect Set </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Greeting19 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules Collect as String Set </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect as String List </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SmartRules Collect as String List </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect List </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Greeting23 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SimpleRules Collect List </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting22</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rules String </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Greeting70</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> (Integer hour)</t>
-    </r>
-  </si>
-  <si>
-    <t>=null</t>
+      <t xml:space="preserve"> (String arg0, String carBrand, String carModel, String country)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="\ &quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2697,7 +2762,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -3223,12 +3288,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC91D"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3464,6 +3666,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3473,22 +3681,58 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="47" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="49" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="50" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="51" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="53" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="54" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="55" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 5" xfId="1"/>
+    <cellStyle name="Обычный 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3882,15 +4126,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78:E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8.140625" style="1" customWidth="1" collapsed="1"/>
@@ -3906,13 +4150,13 @@
     <col min="12" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="13.5" thickBot="1">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3923,7 +4167,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="80" t="s">
@@ -3933,12 +4177,12 @@
       <c r="E4" s="82"/>
       <c r="F4" s="5"/>
       <c r="G4" s="80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" s="81"/>
       <c r="I4" s="82"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="22.5" customHeight="1">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="35" t="s">
@@ -3961,7 +4205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="35" t="s">
@@ -3981,10 +4225,10 @@
         <v>2</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="35" t="s">
@@ -4007,7 +4251,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="12.75" customHeight="1">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="35" t="s">
@@ -4030,7 +4274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="38" t="s">
@@ -4053,7 +4297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="13.5" thickTop="1">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="41">
@@ -4076,7 +4320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="43">
@@ -4099,7 +4343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="43">
@@ -4122,7 +4366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="13.5" thickBot="1">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="46">
@@ -4145,7 +4389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -4156,9 +4400,9 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1"/>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="17" spans="1:11" s="5" customFormat="1">
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:11" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C17" s="80" t="s">
         <v>78</v>
       </c>
@@ -4166,13 +4410,13 @@
       <c r="E17" s="81"/>
       <c r="F17" s="82"/>
       <c r="H17" s="80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I17" s="81"/>
       <c r="J17" s="81"/>
       <c r="K17" s="82"/>
     </row>
-    <row r="18" spans="1:11" s="5" customFormat="1" ht="25.5">
+    <row r="18" spans="1:11" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="C18" s="35" t="s">
         <v>29</v>
       </c>
@@ -4198,7 +4442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="5" customFormat="1">
+    <row r="19" spans="1:11" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C19" s="35" t="s">
         <v>1</v>
       </c>
@@ -4218,13 +4462,13 @@
         <v>2</v>
       </c>
       <c r="J19" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="5" customFormat="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C20" s="35" t="s">
         <v>3</v>
       </c>
@@ -4250,7 +4494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="35" t="s">
@@ -4279,7 +4523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="2" customFormat="1" ht="13.5" thickBot="1">
+    <row r="22" spans="1:11" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="38" t="s">
@@ -4308,7 +4552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" ht="13.5" thickTop="1">
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="41">
@@ -4333,7 +4577,7 @@
       </c>
       <c r="K23" s="42"/>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1">
+    <row r="24" spans="1:11" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="43">
@@ -4358,7 +4602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="3" customFormat="1">
+    <row r="25" spans="1:11" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="43">
@@ -4383,7 +4627,7 @@
       </c>
       <c r="K25" s="45"/>
     </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="46">
@@ -4408,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1">
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -4418,7 +4662,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:11" s="3" customFormat="1">
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -4428,14 +4672,14 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:11" s="3" customFormat="1" ht="15.75">
+    <row r="30" spans="1:11" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="80" t="s">
@@ -4444,7 +4688,7 @@
       <c r="D30" s="81"/>
       <c r="E30" s="82"/>
     </row>
-    <row r="31" spans="1:11" s="3" customFormat="1">
+    <row r="31" spans="1:11" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="35" t="s">
@@ -4457,7 +4701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="35" t="s">
@@ -4468,7 +4712,7 @@
       </c>
       <c r="E32" s="37"/>
     </row>
-    <row r="33" spans="1:10" s="3" customFormat="1" ht="15.75">
+    <row r="33" spans="1:10" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="35" t="s">
@@ -4479,12 +4723,12 @@
       </c>
       <c r="E33" s="37"/>
       <c r="H33" s="80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I33" s="81"/>
       <c r="J33" s="82"/>
     </row>
-    <row r="34" spans="1:10" s="3" customFormat="1" ht="26.25" thickBot="1">
+    <row r="34" spans="1:10" s="3" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="38" t="s">
@@ -4506,7 +4750,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" ht="13.5" thickTop="1">
+    <row r="35" spans="1:10" s="3" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="41" t="s">
@@ -4528,7 +4772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="3" customFormat="1">
+    <row r="36" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="43" t="s">
@@ -4548,7 +4792,7 @@
       </c>
       <c r="J36" s="37"/>
     </row>
-    <row r="37" spans="1:10" s="3" customFormat="1">
+    <row r="37" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="43" t="s">
@@ -4570,7 +4814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="38" spans="1:10" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="43" t="s">
@@ -4592,7 +4836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="3" customFormat="1" ht="14.25" thickTop="1" thickBot="1">
+    <row r="39" spans="1:10" s="3" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="52" t="s">
@@ -4609,10 +4853,10 @@
         <v>11</v>
       </c>
       <c r="J39" s="42" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="3" customFormat="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -4628,7 +4872,7 @@
       </c>
       <c r="J40" s="45"/>
     </row>
-    <row r="41" spans="1:10" s="3" customFormat="1">
+    <row r="41" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -4646,7 +4890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="3" customFormat="1" ht="13.5" thickBot="1">
+    <row r="42" spans="1:10" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -4664,7 +4908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="3" customFormat="1">
+    <row r="43" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="80" t="s">
@@ -4676,7 +4920,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:10" s="3" customFormat="1">
+    <row r="44" spans="1:10" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="35" t="s">
@@ -4694,7 +4938,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:10" s="5" customFormat="1">
+    <row r="45" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C45" s="35" t="s">
         <v>15</v>
       </c>
@@ -4704,7 +4948,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="37"/>
     </row>
-    <row r="46" spans="1:10" s="2" customFormat="1">
+    <row r="46" spans="1:10" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="35" t="s">
@@ -4718,7 +4962,7 @@
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" ht="13.5" thickBot="1">
+    <row r="47" spans="1:10" s="2" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="38" t="s">
@@ -4736,7 +4980,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:10" s="5" customFormat="1" ht="13.5" thickTop="1">
+    <row r="48" spans="1:10" s="5" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C48" s="41" t="s">
         <v>18</v>
       </c>
@@ -4750,7 +4994,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="5" customFormat="1">
+    <row r="49" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C49" s="43" t="s">
         <v>18</v>
       </c>
@@ -4762,7 +5006,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="5" customFormat="1">
+    <row r="50" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C50" s="43" t="s">
         <v>21</v>
       </c>
@@ -4774,7 +5018,7 @@
       </c>
       <c r="F50" s="51"/>
     </row>
-    <row r="51" spans="1:15" s="5" customFormat="1">
+    <row r="51" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C51" s="43" t="s">
         <v>21</v>
       </c>
@@ -4786,7 +5030,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1">
+    <row r="52" spans="1:15" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="46" t="s">
         <v>22</v>
       </c>
@@ -4796,10 +5040,10 @@
         <v>500</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="5" customFormat="1"/>
-    <row r="54" spans="1:15" s="5" customFormat="1"/>
-    <row r="55" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="56" spans="1:15" s="2" customFormat="1" ht="15.75">
+    <row r="53" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:15" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:15" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="80" t="s">
@@ -4811,7 +5055,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:15" s="2" customFormat="1">
+    <row r="57" spans="1:15" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="35" t="s">
@@ -4832,7 +5076,7 @@
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
     </row>
-    <row r="58" spans="1:15" s="2" customFormat="1">
+    <row r="58" spans="1:15" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="35"/>
@@ -4849,7 +5093,7 @@
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
     </row>
-    <row r="59" spans="1:15" s="5" customFormat="1">
+    <row r="59" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C59" s="35"/>
       <c r="D59" s="30" t="s">
         <v>35</v>
@@ -4859,7 +5103,7 @@
       </c>
       <c r="F59" s="37"/>
     </row>
-    <row r="60" spans="1:15" s="5" customFormat="1" ht="13.5" thickBot="1">
+    <row r="60" spans="1:15" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="38" t="s">
         <v>28</v>
       </c>
@@ -4873,7 +5117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="5" customFormat="1" ht="13.5" thickTop="1">
+    <row r="61" spans="1:15" s="5" customFormat="1" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C61" s="57" t="s">
         <v>23</v>
       </c>
@@ -4887,7 +5131,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="5" customFormat="1">
+    <row r="62" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C62" s="59" t="s">
         <v>24</v>
       </c>
@@ -4899,7 +5143,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="5" customFormat="1">
+    <row r="63" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C63" s="59" t="s">
         <v>25</v>
       </c>
@@ -4913,7 +5157,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="5" customFormat="1">
+    <row r="64" spans="1:15" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="C64" s="59" t="s">
         <v>26</v>
       </c>
@@ -4925,7 +5169,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1">
+    <row r="65" spans="1:14" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="61" t="s">
         <v>27</v>
       </c>
@@ -4937,8 +5181,8 @@
         <v>500</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="5" customFormat="1"/>
-    <row r="67" spans="1:14">
+    <row r="66" spans="1:14" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -4948,7 +5192,7 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
     </row>
-    <row r="68" spans="1:14" ht="13.5" thickBot="1">
+    <row r="68" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -4958,7 +5202,7 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75">
+    <row r="69" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="80" t="s">
@@ -4970,7 +5214,7 @@
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
     </row>
-    <row r="70" spans="1:14" ht="13.5" thickBot="1">
+    <row r="70" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="38" t="s">
@@ -4986,7 +5230,7 @@
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="1:14" ht="13.5" thickTop="1">
+    <row r="71" spans="1:14" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="41" t="s">
@@ -5002,7 +5246,7 @@
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="43" t="s">
@@ -5018,7 +5262,7 @@
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="43" t="s">
@@ -5034,7 +5278,7 @@
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="43" t="s">
@@ -5051,7 +5295,7 @@
       <c r="H74" s="5"/>
       <c r="N74" s="4"/>
     </row>
-    <row r="75" spans="1:14" ht="13.5" thickBot="1">
+    <row r="75" spans="1:14" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="52" t="s">
@@ -5066,7 +5310,7 @@
       <c r="H75" s="5"/>
       <c r="N75" s="4"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -5077,15 +5321,15 @@
       <c r="H76" s="5"/>
       <c r="N76" s="3"/>
     </row>
-    <row r="77" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1"/>
-    <row r="78" spans="1:14" s="5" customFormat="1" ht="15.75">
+    <row r="77" spans="1:14" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:14" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C78" s="80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D78" s="81"/>
       <c r="E78" s="82"/>
     </row>
-    <row r="79" spans="1:14" s="5" customFormat="1" ht="13.5" thickBot="1">
+    <row r="79" spans="1:14" s="5" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="38" t="s">
         <v>16</v>
       </c>
@@ -5096,7 +5340,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="13.5" thickTop="1">
+    <row r="80" spans="1:14" ht="14.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="41" t="s">
@@ -5114,7 +5358,7 @@
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="43" t="s">
@@ -5132,7 +5376,7 @@
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="43" t="s">
@@ -5150,7 +5394,7 @@
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="43" t="s">
@@ -5169,7 +5413,7 @@
       <c r="J83" s="5"/>
       <c r="M83" s="4"/>
     </row>
-    <row r="84" spans="1:13" ht="13.5" thickBot="1">
+    <row r="84" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="52" t="s">
@@ -5186,7 +5430,7 @@
       <c r="J84" s="5"/>
       <c r="M84" s="3"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -5199,7 +5443,7 @@
       <c r="J85" s="5"/>
       <c r="M85" s="3"/>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -5212,7 +5456,7 @@
       <c r="J86" s="5"/>
       <c r="M86" s="3"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -5225,7 +5469,7 @@
       <c r="J87" s="5"/>
       <c r="M87" s="3"/>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -5238,7 +5482,7 @@
       <c r="J88" s="5"/>
       <c r="M88" s="3"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -5250,17 +5494,17 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:13" s="5" customFormat="1"/>
-    <row r="91" spans="1:13" s="5" customFormat="1"/>
-    <row r="92" spans="1:13" s="5" customFormat="1"/>
-    <row r="93" spans="1:13" s="5" customFormat="1"/>
-    <row r="94" spans="1:13" s="5" customFormat="1"/>
-    <row r="95" spans="1:13" s="5" customFormat="1"/>
-    <row r="96" spans="1:13" s="5" customFormat="1"/>
-    <row r="97" spans="1:10" s="5" customFormat="1"/>
-    <row r="98" spans="1:10" s="5" customFormat="1"/>
-    <row r="99" spans="1:10" s="5" customFormat="1"/>
-    <row r="100" spans="1:10">
+    <row r="90" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:13" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -5272,34 +5516,34 @@
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="1:10" s="5" customFormat="1"/>
-    <row r="102" spans="1:10" s="5" customFormat="1"/>
-    <row r="103" spans="1:10" s="5" customFormat="1"/>
-    <row r="104" spans="1:10" s="5" customFormat="1"/>
-    <row r="105" spans="1:10" s="5" customFormat="1"/>
-    <row r="106" spans="1:10" s="5" customFormat="1"/>
-    <row r="107" spans="1:10" s="5" customFormat="1"/>
-    <row r="108" spans="1:10" s="5" customFormat="1"/>
-    <row r="109" spans="1:10" s="5" customFormat="1"/>
-    <row r="110" spans="1:10" s="5" customFormat="1"/>
-    <row r="111" spans="1:10" s="5" customFormat="1"/>
-    <row r="112" spans="1:10" s="5" customFormat="1"/>
-    <row r="113" spans="1:10" s="5" customFormat="1"/>
-    <row r="114" spans="1:10" s="5" customFormat="1"/>
-    <row r="115" spans="1:10" s="5" customFormat="1"/>
-    <row r="116" spans="1:10" s="5" customFormat="1"/>
-    <row r="117" spans="1:10" s="5" customFormat="1"/>
-    <row r="118" spans="1:10" s="5" customFormat="1"/>
-    <row r="119" spans="1:10" s="5" customFormat="1"/>
-    <row r="120" spans="1:10" s="5" customFormat="1"/>
-    <row r="121" spans="1:10" s="5" customFormat="1"/>
-    <row r="122" spans="1:10" s="5" customFormat="1"/>
-    <row r="123" spans="1:10" s="5" customFormat="1"/>
-    <row r="124" spans="1:10" s="5" customFormat="1"/>
-    <row r="125" spans="1:10" s="5" customFormat="1"/>
-    <row r="126" spans="1:10" s="5" customFormat="1"/>
-    <row r="127" spans="1:10" s="5" customFormat="1"/>
-    <row r="128" spans="1:10">
+    <row r="101" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:10" s="5" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
@@ -5311,7 +5555,7 @@
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
@@ -5323,7 +5567,7 @@
       <c r="I129" s="5"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
@@ -5335,7 +5579,7 @@
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
@@ -5347,7 +5591,7 @@
       <c r="I131" s="5"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
@@ -5361,6 +5605,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C69:E69"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:E30"/>
@@ -5368,11 +5617,6 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H33:J33"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="C69:E69"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5382,14 +5626,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B5:I60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="43" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5398,15 +5642,20 @@
     <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5" ht="13.5" thickBot="1"/>
-    <row r="6" spans="3:5" ht="15.75">
+    <row r="5" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="3:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C6" s="80" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="82"/>
-    </row>
-    <row r="7" spans="3:5">
+      <c r="G6" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="81"/>
+      <c r="I6" s="82"/>
+    </row>
+    <row r="7" spans="3:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="35" t="s">
         <v>1</v>
       </c>
@@ -5416,8 +5665,17 @@
       <c r="E7" s="37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="3:5">
+      <c r="G7" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C8" s="35" t="s">
         <v>15</v>
       </c>
@@ -5425,8 +5683,17 @@
         <v>68</v>
       </c>
       <c r="E8" s="37"/>
-    </row>
-    <row r="9" spans="3:5">
+      <c r="G8" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="19">
+        <v>700</v>
+      </c>
+      <c r="I8" s="58">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C9" s="35" t="s">
         <v>35</v>
       </c>
@@ -5434,8 +5701,17 @@
         <v>35</v>
       </c>
       <c r="E9" s="37"/>
-    </row>
-    <row r="10" spans="3:5" ht="12" customHeight="1" thickBot="1">
+      <c r="G9" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="10">
+        <v>300</v>
+      </c>
+      <c r="I9" s="60">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="64" t="s">
         <v>40</v>
       </c>
@@ -5445,8 +5721,15 @@
       <c r="E10" s="66" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" ht="13.5" thickTop="1">
+      <c r="G10" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="85">
+        <v>500</v>
+      </c>
+      <c r="I10" s="86"/>
+    </row>
+    <row r="11" spans="3:9" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C11" s="43" t="s">
         <v>18</v>
       </c>
@@ -5457,7 +5740,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C12" s="43" t="s">
         <v>21</v>
       </c>
@@ -5468,29 +5751,29 @@
         <v>350</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="13.5" thickBot="1">
+    <row r="13" spans="3:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="88">
+      <c r="D13" s="85">
         <v>500</v>
       </c>
-      <c r="E13" s="89"/>
-    </row>
-    <row r="16" spans="3:5" ht="13.5" thickBot="1"/>
-    <row r="17" spans="3:9" ht="15.75">
+      <c r="E13" s="86"/>
+    </row>
+    <row r="16" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="3:9" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C17" s="80" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="81"/>
       <c r="E17" s="82"/>
       <c r="G17" s="80" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="H17" s="81"/>
       <c r="I17" s="82"/>
     </row>
-    <row r="18" spans="3:9" ht="26.25" thickBot="1">
+    <row r="18" spans="3:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="64" t="s">
         <v>40</v>
       </c>
@@ -5510,7 +5793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:9" ht="13.5" thickTop="1">
+    <row r="19" spans="3:9" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C19" s="43" t="s">
         <v>18</v>
       </c>
@@ -5530,7 +5813,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="3:9">
+    <row r="20" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C20" s="43" t="s">
         <v>21</v>
       </c>
@@ -5550,46 +5833,46 @@
         <v>350</v>
       </c>
     </row>
-    <row r="21" spans="3:9" ht="13.5" thickBot="1">
+    <row r="21" spans="3:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="88">
+      <c r="D21" s="85">
         <v>500</v>
       </c>
-      <c r="E21" s="89"/>
+      <c r="E21" s="86"/>
       <c r="G21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="88">
+      <c r="H21" s="85">
         <v>500</v>
       </c>
-      <c r="I21" s="89"/>
-    </row>
-    <row r="25" spans="3:9" ht="15.75">
-      <c r="C25" s="85" t="s">
+      <c r="I21" s="86"/>
+    </row>
+    <row r="25" spans="3:9" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C25" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-    </row>
-    <row r="26" spans="3:9">
-      <c r="C26" s="86" t="s">
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+    </row>
+    <row r="26" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C26" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87" t="s">
+      <c r="E26" s="89"/>
+      <c r="F26" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="87"/>
-    </row>
-    <row r="27" spans="3:9" ht="13.5" thickBot="1">
-      <c r="C27" s="86"/>
+      <c r="G26" s="89"/>
+    </row>
+    <row r="27" spans="3:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="88"/>
       <c r="D27" s="18" t="s">
         <v>44</v>
       </c>
@@ -5603,7 +5886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="3:9" ht="13.5" thickTop="1">
+    <row r="28" spans="3:9" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C28" s="7" t="s">
         <v>37</v>
       </c>
@@ -5620,7 +5903,7 @@
         <v>91030</v>
       </c>
     </row>
-    <row r="29" spans="3:9">
+    <row r="29" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C29" s="7" t="s">
         <v>38</v>
       </c>
@@ -5637,7 +5920,7 @@
         <v>93220</v>
       </c>
     </row>
-    <row r="30" spans="3:9">
+    <row r="30" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C30" s="7" t="s">
         <v>41</v>
       </c>
@@ -5654,7 +5937,7 @@
         <v>110030</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="13.5" thickBot="1">
+    <row r="31" spans="3:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="s">
         <v>42</v>
       </c>
@@ -5671,31 +5954,31 @@
         <v>130030</v>
       </c>
     </row>
-    <row r="32" spans="3:9" ht="13.5" thickTop="1"/>
-    <row r="34" spans="3:7" ht="15.75">
-      <c r="C34" s="85" t="s">
+    <row r="32" spans="3:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C34" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-    </row>
-    <row r="35" spans="3:7">
-      <c r="C35" s="86" t="s">
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+    </row>
+    <row r="35" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C35" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="87" t="s">
+      <c r="D35" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87" t="s">
+      <c r="E35" s="89"/>
+      <c r="F35" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="87"/>
-    </row>
-    <row r="36" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C36" s="86"/>
+      <c r="G35" s="89"/>
+    </row>
+    <row r="36" spans="3:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="88"/>
       <c r="D36" s="18" t="s">
         <v>44</v>
       </c>
@@ -5709,7 +5992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="3:7" ht="13.5" thickTop="1">
+    <row r="37" spans="3:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C37" s="7" t="s">
         <v>37</v>
       </c>
@@ -5726,7 +6009,7 @@
         <v>91030</v>
       </c>
     </row>
-    <row r="38" spans="3:7">
+    <row r="38" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C38" s="7" t="s">
         <v>38</v>
       </c>
@@ -5743,7 +6026,7 @@
         <v>93220</v>
       </c>
     </row>
-    <row r="39" spans="3:7">
+    <row r="39" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C39" s="7" t="s">
         <v>41</v>
       </c>
@@ -5760,7 +6043,7 @@
         <v>110030</v>
       </c>
     </row>
-    <row r="40" spans="3:7" ht="13.5" thickBot="1">
+    <row r="40" spans="3:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C40" s="8" t="s">
         <v>42</v>
       </c>
@@ -5777,14 +6060,180 @@
         <v>130030</v>
       </c>
     </row>
-    <row r="41" spans="3:7" ht="13.5" thickTop="1"/>
+    <row r="41" spans="3:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C44" s="92" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="93"/>
+    </row>
+    <row r="45" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C45" s="94" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="95"/>
+      <c r="F45" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" s="96"/>
+    </row>
+    <row r="46" spans="3:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="94"/>
+      <c r="D46" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="97" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="19">
+        <v>55150</v>
+      </c>
+      <c r="E47" s="20">
+        <v>47350</v>
+      </c>
+      <c r="F47" s="20">
+        <v>105630</v>
+      </c>
+      <c r="G47" s="99">
+        <v>91030</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C48" s="98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="10">
+        <v>57150</v>
+      </c>
+      <c r="E48" s="9">
+        <v>49350</v>
+      </c>
+      <c r="F48" s="9">
+        <v>107630</v>
+      </c>
+      <c r="G48" s="100">
+        <v>93220</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C49" s="98" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="11">
+        <v>64400</v>
+      </c>
+      <c r="E49" s="12">
+        <v>57150</v>
+      </c>
+      <c r="F49" s="12">
+        <v>125600</v>
+      </c>
+      <c r="G49" s="101">
+        <v>110030</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="C50" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="103">
+        <v>90400</v>
+      </c>
+      <c r="E50" s="104">
+        <v>83500</v>
+      </c>
+      <c r="F50" s="104">
+        <v>145600</v>
+      </c>
+      <c r="G50" s="105">
+        <v>130030</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C25:G25"/>
+  <mergeCells count="20">
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:E35"/>
@@ -5794,6 +6243,13 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5801,14 +6257,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:M105"/>
   <sheetViews>
-    <sheetView topLeftCell="B82" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25" customWidth="1" collapsed="1"/>
@@ -5822,8 +6278,8 @@
     <col min="13" max="13" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="13.5" thickBot="1"/>
-    <row r="5" spans="3:10" ht="15.75">
+    <row r="4" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C5" s="80" t="s">
         <v>64</v>
       </c>
@@ -5835,7 +6291,7 @@
       <c r="I5" s="81"/>
       <c r="J5" s="82"/>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C6" s="35" t="s">
         <v>1</v>
       </c>
@@ -5861,7 +6317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="13.5" thickBot="1">
+    <row r="7" spans="3:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
@@ -5887,7 +6343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
+    <row r="8" spans="3:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="69" t="s">
         <v>13</v>
       </c>
@@ -5913,7 +6369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
+    <row r="9" spans="3:10" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="71"/>
       <c r="D9" s="72"/>
       <c r="E9" s="72"/>
@@ -5923,15 +6379,15 @@
       <c r="I9" s="72"/>
       <c r="J9" s="74"/>
     </row>
-    <row r="12" spans="3:10" ht="13.5" thickBot="1"/>
-    <row r="13" spans="3:10" ht="15.75">
+    <row r="12" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="3:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C13" s="80" t="s">
         <v>65</v>
       </c>
       <c r="D13" s="81"/>
       <c r="E13" s="82"/>
     </row>
-    <row r="14" spans="3:10">
+    <row r="14" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C14" s="90" t="s">
         <v>1</v>
       </c>
@@ -5940,7 +6396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
+    <row r="15" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C15" s="90" t="s">
         <v>48</v>
       </c>
@@ -5949,7 +6405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C16" s="35" t="s">
         <v>30</v>
       </c>
@@ -5960,7 +6416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:5" ht="13.5" thickBot="1">
+    <row r="17" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C17" s="38" t="s">
         <v>5</v>
       </c>
@@ -5971,7 +6427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:5" ht="13.5" thickTop="1">
+    <row r="18" spans="3:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C18" s="41">
         <v>0</v>
       </c>
@@ -5982,7 +6438,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C19" s="43">
         <v>12</v>
       </c>
@@ -5993,7 +6449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C20" s="43">
         <v>18</v>
       </c>
@@ -6004,7 +6460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="3:5" ht="13.5" thickBot="1">
+    <row r="21" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="46">
         <v>22</v>
       </c>
@@ -6015,14 +6471,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="3:5" ht="13.5" thickBot="1"/>
-    <row r="25" spans="3:5" ht="15.75">
+    <row r="24" spans="3:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C25" s="80" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="82"/>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C26" s="35" t="s">
         <v>1</v>
       </c>
@@ -6030,7 +6486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C27" s="35" t="s">
         <v>54</v>
       </c>
@@ -6038,7 +6494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C28" s="35" t="s">
         <v>55</v>
       </c>
@@ -6046,7 +6502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="3:5" ht="13.5" thickBot="1">
+    <row r="29" spans="3:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="38" t="s">
         <v>53</v>
       </c>
@@ -6054,7 +6510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="3:5" ht="13.5" thickTop="1">
+    <row r="30" spans="3:5" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C30" s="41" t="s">
         <v>49</v>
       </c>
@@ -6062,7 +6518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C31" s="43" t="s">
         <v>50</v>
       </c>
@@ -6070,7 +6526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" spans="3:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C32" s="43" t="s">
         <v>51</v>
       </c>
@@ -6078,7 +6534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="3:13" ht="13.5" thickBot="1">
+    <row r="33" spans="3:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="75" t="s">
         <v>52</v>
       </c>
@@ -6086,8 +6542,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="3:13" ht="13.5" thickBot="1"/>
-    <row r="37" spans="3:13" ht="15.75">
+    <row r="36" spans="3:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="3:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C37" s="80" t="s">
         <v>67</v>
       </c>
@@ -6097,15 +6553,15 @@
       </c>
       <c r="G37" s="82"/>
       <c r="I37" s="80" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J37" s="82"/>
       <c r="L37" s="80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M37" s="82"/>
     </row>
-    <row r="38" spans="3:13" ht="13.5" thickBot="1">
+    <row r="38" spans="3:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="38" t="s">
         <v>53</v>
       </c>
@@ -6131,7 +6587,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="3:13" ht="13.5" thickTop="1">
+    <row r="39" spans="3:13" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C39" s="41" t="s">
         <v>49</v>
       </c>
@@ -6157,7 +6613,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="3:13">
+    <row r="40" spans="3:13" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C40" s="43" t="s">
         <v>50</v>
       </c>
@@ -6171,19 +6627,19 @@
         <v>57</v>
       </c>
       <c r="I40" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J40" s="45" t="s">
         <v>57</v>
       </c>
       <c r="L40" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M40" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="3:13">
+    <row r="41" spans="3:13" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C41" s="43" t="s">
         <v>51</v>
       </c>
@@ -6197,19 +6653,19 @@
         <v>58</v>
       </c>
       <c r="I41" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J41" s="45" t="s">
         <v>58</v>
       </c>
       <c r="L41" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M41" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="3:13" ht="13.5" thickBot="1">
+    <row r="42" spans="3:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C42" s="75" t="s">
         <v>52</v>
       </c>
@@ -6235,22 +6691,22 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="3:13" ht="13.5" thickBot="1"/>
-    <row r="46" spans="3:13" ht="15.75">
+    <row r="45" spans="3:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="3:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C46" s="80" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="82"/>
       <c r="F46" s="80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G46" s="82"/>
       <c r="I46" s="80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J46" s="82"/>
     </row>
-    <row r="47" spans="3:13" ht="13.5" thickBot="1">
+    <row r="47" spans="3:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C47" s="35" t="s">
         <v>1</v>
       </c>
@@ -6270,7 +6726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="3:13" ht="26.25" thickTop="1">
+    <row r="48" spans="3:13" ht="27.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C48" s="35" t="s">
         <v>54</v>
       </c>
@@ -6290,7 +6746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="3:10">
+    <row r="49" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C49" s="35" t="s">
         <v>55</v>
       </c>
@@ -6298,19 +6754,19 @@
         <v>11</v>
       </c>
       <c r="F49" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" s="45" t="s">
         <v>57</v>
       </c>
       <c r="I49" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J49" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="3:10" ht="13.5" thickBot="1">
+    <row r="50" spans="3:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C50" s="38" t="s">
         <v>53</v>
       </c>
@@ -6318,19 +6774,19 @@
         <v>12</v>
       </c>
       <c r="F50" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G50" s="45" t="s">
         <v>58</v>
       </c>
       <c r="I50" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J50" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="3:10" ht="14.25" thickTop="1" thickBot="1">
+    <row r="51" spans="3:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C51" s="41" t="s">
         <v>49</v>
       </c>
@@ -6350,7 +6806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="3:10">
+    <row r="52" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C52" s="43" t="s">
         <v>50</v>
       </c>
@@ -6358,7 +6814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="3:10">
+    <row r="53" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="C53" s="43" t="s">
         <v>51</v>
       </c>
@@ -6366,7 +6822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="3:10" ht="13.5" thickBot="1">
+    <row r="54" spans="3:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C54" s="75" t="s">
         <v>52</v>
       </c>
@@ -6374,17 +6830,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="3:10" ht="15.75">
+    <row r="55" spans="3:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F55" s="80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G55" s="82"/>
       <c r="I55" s="80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J55" s="82"/>
     </row>
-    <row r="56" spans="3:10" ht="13.5" thickBot="1">
+    <row r="56" spans="3:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F56" s="38" t="s">
         <v>53</v>
       </c>
@@ -6398,7 +6854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="3:10" ht="13.5" thickTop="1">
+    <row r="57" spans="3:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F57" s="41" t="s">
         <v>49</v>
       </c>
@@ -6412,35 +6868,35 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="3:10">
+    <row r="58" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F58" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G58" s="45" t="s">
         <v>57</v>
       </c>
       <c r="I58" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J58" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="3:10">
+    <row r="59" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F59" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G59" s="45" t="s">
         <v>58</v>
       </c>
       <c r="I59" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J59" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="3:10" ht="13.5" thickBot="1">
+    <row r="60" spans="3:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F60" s="75" t="s">
         <v>52</v>
       </c>
@@ -6454,18 +6910,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="3:10" ht="13.5" thickBot="1"/>
-    <row r="64" spans="3:10" ht="15.75">
+    <row r="63" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="3:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F64" s="80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G64" s="82"/>
       <c r="I64" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J64" s="82"/>
     </row>
-    <row r="65" spans="6:10" ht="13.5" thickBot="1">
+    <row r="65" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F65" s="38" t="s">
         <v>53</v>
       </c>
@@ -6479,7 +6935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="6:10" ht="13.5" thickTop="1">
+    <row r="66" spans="6:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F66" s="41" t="s">
         <v>49</v>
       </c>
@@ -6493,35 +6949,35 @@
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="6:10">
+    <row r="67" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F67" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G67" s="45" t="s">
         <v>57</v>
       </c>
       <c r="I67" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J67" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="6:10">
+    <row r="68" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F68" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G68" s="45" t="s">
         <v>58</v>
       </c>
       <c r="I68" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J68" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="6:10" ht="13.5" thickBot="1">
+    <row r="69" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F69" s="75" t="s">
         <v>52</v>
       </c>
@@ -6535,19 +6991,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="6:10" ht="13.5" thickBot="1"/>
-    <row r="73" spans="6:10" ht="15.75">
+    <row r="72" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="6:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F73" s="80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G73" s="82"/>
       <c r="H73" s="3"/>
       <c r="I73" s="80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J73" s="82"/>
     </row>
-    <row r="74" spans="6:10" ht="13.5" thickBot="1">
+    <row r="74" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F74" s="38" t="s">
         <v>53</v>
       </c>
@@ -6562,7 +7018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="6:10" ht="13.5" thickTop="1">
+    <row r="75" spans="6:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F75" s="41" t="s">
         <v>49</v>
       </c>
@@ -6577,37 +7033,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="6:10">
+    <row r="76" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F76" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G76" s="45" t="s">
         <v>56</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J76" s="45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="6:10">
+    <row r="77" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F77" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G77" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J77" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="6:10" ht="13.5" thickBot="1">
+    <row r="78" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F78" s="75" t="s">
         <v>52</v>
       </c>
@@ -6622,39 +7078,39 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="6:10">
+    <row r="79" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="6:10">
+    <row r="80" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="6:10" ht="13.5" thickBot="1">
+    <row r="81" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="6:10" ht="15.75">
+    <row r="82" spans="6:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F82" s="80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G82" s="82"/>
       <c r="H82" s="3"/>
       <c r="I82" s="80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J82" s="82"/>
     </row>
-    <row r="83" spans="6:10" ht="13.5" thickBot="1">
+    <row r="83" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F83" s="38" t="s">
         <v>53</v>
       </c>
@@ -6669,7 +7125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="6:10" ht="13.5" thickTop="1">
+    <row r="84" spans="6:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F84" s="41" t="s">
         <v>49</v>
       </c>
@@ -6684,37 +7140,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="6:10">
+    <row r="85" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F85" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G85" s="45" t="s">
         <v>56</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J85" s="45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="6:10">
+    <row r="86" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F86" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G86" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J86" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="6:10" ht="13.5" thickBot="1">
+    <row r="87" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F87" s="75" t="s">
         <v>52</v>
       </c>
@@ -6729,19 +7185,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="6:10" ht="13.5" thickBot="1"/>
-    <row r="91" spans="6:10" ht="15.75">
+    <row r="90" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="6:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F91" s="80" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G91" s="82"/>
       <c r="H91" s="3"/>
       <c r="I91" s="80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J91" s="82"/>
     </row>
-    <row r="92" spans="6:10" ht="13.5" thickBot="1">
+    <row r="92" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F92" s="38" t="s">
         <v>53</v>
       </c>
@@ -6756,7 +7212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="6:10" ht="13.5" thickTop="1">
+    <row r="93" spans="6:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F93" s="41" t="s">
         <v>49</v>
       </c>
@@ -6771,37 +7227,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="6:10">
+    <row r="94" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F94" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G94" s="45" t="s">
         <v>57</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J94" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="6:10">
+    <row r="95" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F95" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G95" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J95" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="6:10" ht="13.5" thickBot="1">
+    <row r="96" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F96" s="75" t="s">
         <v>52</v>
       </c>
@@ -6816,39 +7272,39 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="6:10">
+    <row r="97" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="6:10">
+    <row r="98" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="6:10" ht="13.5" thickBot="1">
+    <row r="99" spans="6:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="6:10" ht="15.75">
+    <row r="100" spans="6:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F100" s="80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G100" s="82"/>
       <c r="H100" s="3"/>
       <c r="I100" s="80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J100" s="82"/>
     </row>
-    <row r="101" spans="6:10" ht="13.5" thickBot="1">
+    <row r="101" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F101" s="38" t="s">
         <v>53</v>
       </c>
@@ -6863,7 +7319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="6:10" ht="13.5" thickTop="1">
+    <row r="102" spans="6:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F102" s="41" t="s">
         <v>49</v>
       </c>
@@ -6878,37 +7334,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="6:10">
+    <row r="103" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F103" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G103" s="45" t="s">
         <v>57</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J103" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="104" spans="6:10">
+    <row r="104" spans="6:10" ht="13.5" x14ac:dyDescent="0.2">
       <c r="F104" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G104" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J104" s="45" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="6:10" ht="13.5" thickBot="1">
+    <row r="105" spans="6:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F105" s="75" t="s">
         <v>52</v>
       </c>
@@ -6925,6 +7381,20 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="I55:J55"/>
     <mergeCell ref="F91:G91"/>
     <mergeCell ref="I91:J91"/>
     <mergeCell ref="F100:G100"/>
@@ -6935,20 +7405,6 @@
     <mergeCell ref="I73:J73"/>
     <mergeCell ref="F82:G82"/>
     <mergeCell ref="I82:J82"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="I37:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-8250 Opportunity to use $ruleId/$rule in Rules and SmartRules
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF00E015-09FA-4FDE-AAA4-74143708AB86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B26380-5A65-4102-A149-9B48FDFA64CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="810" windowWidth="31335" windowHeight="18465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="5" r:id="rId1"/>
@@ -2726,13 +2726,13 @@
     <t>String s</t>
   </si>
   <si>
-    <t>driverMaritalStatus == $rule or  s == driverMaritalStatus</t>
-  </si>
-  <si>
-    <t>greeting + ", World!" + " ruleNumber:" + $ruleId</t>
-  </si>
-  <si>
-    <t>$rule + ": " + ret</t>
+    <t>driverMaritalStatus == $Rule or  s == driverMaritalStatus</t>
+  </si>
+  <si>
+    <t>$Rule + ": " + ret</t>
+  </si>
+  <si>
+    <t>greeting + ", World!" + " ruleNumber:" + $RuleId</t>
   </si>
 </sst>
 </file>
@@ -3841,15 +3841,6 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="59" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3859,6 +3850,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3869,6 +3863,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4279,7 +4279,7 @@
   <dimension ref="A1:Q133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5600,7 +5600,7 @@
         <v>113</v>
       </c>
       <c r="F95" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:13" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
@@ -5792,11 +5792,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C93:F93"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="F100:F101"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:E30"/>
@@ -5804,12 +5805,11 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H33:J33"/>
-    <mergeCell ref="C93:F93"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="D100:D102"/>
-    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C69:E69"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5822,7 +5822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C5:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -5917,10 +5917,10 @@
       <c r="G10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="93">
+      <c r="H10" s="101">
         <v>500</v>
       </c>
-      <c r="I10" s="94"/>
+      <c r="I10" s="102"/>
     </row>
     <row r="11" spans="3:9" ht="14.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C11" s="40" t="s">
@@ -5948,10 +5948,10 @@
       <c r="C13" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="93">
+      <c r="D13" s="101">
         <v>500</v>
       </c>
-      <c r="E13" s="94"/>
+      <c r="E13" s="102"/>
     </row>
     <row r="16" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="3:9" ht="16.5" x14ac:dyDescent="0.2">
@@ -6030,42 +6030,42 @@
       <c r="C21" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="93">
+      <c r="D21" s="101">
         <v>500</v>
       </c>
-      <c r="E21" s="94"/>
+      <c r="E21" s="102"/>
       <c r="G21" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="93">
+      <c r="H21" s="101">
         <v>500</v>
       </c>
-      <c r="I21" s="94"/>
+      <c r="I21" s="102"/>
     </row>
     <row r="25" spans="3:9" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="96"/>
     </row>
     <row r="26" spans="3:9" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="C26" s="96" t="s">
+      <c r="C26" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="97" t="s">
+      <c r="D26" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97" t="s">
+      <c r="E26" s="94"/>
+      <c r="F26" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="97"/>
+      <c r="G26" s="94"/>
     </row>
     <row r="27" spans="3:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="96"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="15" t="s">
         <v>44</v>
       </c>
@@ -6149,29 +6149,29 @@
     </row>
     <row r="32" spans="3:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C34" s="95" t="s">
+      <c r="C34" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
     </row>
     <row r="35" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="C35" s="96" t="s">
+      <c r="C35" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="97" t="s">
+      <c r="D35" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97" t="s">
+      <c r="E35" s="94"/>
+      <c r="F35" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="97"/>
+      <c r="G35" s="94"/>
     </row>
     <row r="36" spans="3:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="96"/>
+      <c r="C36" s="93"/>
       <c r="D36" s="15" t="s">
         <v>44</v>
       </c>
@@ -6255,29 +6255,29 @@
     </row>
     <row r="41" spans="3:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C44" s="98" t="s">
+      <c r="C44" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="99"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="96"/>
+      <c r="G44" s="97"/>
     </row>
     <row r="45" spans="3:7" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="C45" s="100" t="s">
+      <c r="C45" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="101" t="s">
+      <c r="D45" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="101"/>
-      <c r="F45" s="101" t="s">
+      <c r="E45" s="99"/>
+      <c r="F45" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="G45" s="102"/>
+      <c r="G45" s="100"/>
     </row>
     <row r="46" spans="3:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="100"/>
+      <c r="C46" s="98"/>
       <c r="D46" s="62" t="s">
         <v>44</v>
       </c>
@@ -6361,6 +6361,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="H21:I21"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
@@ -6372,15 +6381,6 @@
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:G35"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="H21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6391,8 +6391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C4:M105"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:H21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="H15" s="104"/>
       <c r="I15" s="34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="3:10" ht="13.5" x14ac:dyDescent="0.2">
@@ -7521,6 +7521,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="I55:J55"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="C13:E13"/>
@@ -7533,21 +7548,6 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="I82:J82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-8637 - Modify the order of matching the input values to horizontal conditions in Smart Lookups
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/dt/DTTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\dt\"/>
     </mc:Choice>
@@ -1548,7 +1548,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="120">
   <si>
     <t>Rule</t>
   </si>
@@ -2733,6 +2733,18 @@
   </si>
   <si>
     <t>greeting + ", World!" + " ruleNumber:" + $RuleId</t>
+  </si>
+  <si>
+    <t>SmartLookup DoubleValue CarPrice2 (String country, String carBrand, String carModel, String arg0)</t>
+  </si>
+  <si>
+    <t>SmartLookup DoubleValue CarPrice3 (String carBrand, String carModel, String country, String arg0)</t>
+  </si>
+  <si>
+    <t>SmartLookup DoubleValue DriverPremium6 ( String driverAge, String mStatus, String name)</t>
+  </si>
+  <si>
+    <t>SmartLookup DoubleValue DriverPremium8 (String mStatus, String driverAge, String name)</t>
   </si>
 </sst>
 </file>
@@ -2799,7 +2811,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -2832,19 +2844,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3572,8 +3584,8 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
   <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4284,18 +4296,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="63.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="53.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="63.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="53.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="12" max="16384" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:9" s="1" customFormat="1" ht="13.5" x14ac:dyDescent="0.25"/>
@@ -5828,11 +5840,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="43" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="3" max="4" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="29.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -5843,7 +5855,7 @@
       <c r="D6" s="83"/>
       <c r="E6" s="84"/>
       <c r="G6" s="82" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="H6" s="83"/>
       <c r="I6" s="84"/>
@@ -5961,7 +5973,7 @@
       <c r="D17" s="83"/>
       <c r="E17" s="84"/>
       <c r="G17" s="82" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="H17" s="83"/>
       <c r="I17" s="84"/>
@@ -6150,7 +6162,7 @@
     <row r="32" spans="3:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C34" s="96" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="D34" s="96"/>
       <c r="E34" s="96"/>
@@ -6256,7 +6268,7 @@
     <row r="41" spans="3:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="3:7" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C44" s="95" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D44" s="96"/>
       <c r="E44" s="96"/>
@@ -6397,16 +6409,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>

</xml_diff>